<commit_message>
additional testcase for clinician
</commit_message>
<xml_diff>
--- a/resources/clinicianToDoVisit.xlsx
+++ b/resources/clinicianToDoVisit.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="177">
   <si>
     <t>/html/body/div/div/md-content/div/section/div[5]/button</t>
   </si>
@@ -451,12 +451,6 @@
   </si>
   <si>
     <t>Sign-in</t>
-  </si>
-  <si>
-    <t>//*[@id="widget"]/div[1]/div[3]</t>
-  </si>
-  <si>
-    <t>Click Notes</t>
   </si>
   <si>
     <t>Save</t>
@@ -948,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -993,10 +987,10 @@
         <v>47</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1004,7 +998,7 @@
         <v>123</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
@@ -1024,7 +1018,7 @@
         <v>124</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -1044,13 +1038,13 @@
         <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -1133,10 +1127,10 @@
     </row>
     <row r="8" spans="1:10" ht="30">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
@@ -1156,7 +1150,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
@@ -1176,7 +1170,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="B10" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
@@ -1196,10 +1190,10 @@
     </row>
     <row r="11" spans="1:10" ht="30">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
@@ -1219,7 +1213,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="B12" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
@@ -1239,7 +1233,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="B13" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -1259,7 +1253,7 @@
     </row>
     <row r="14" spans="1:10" ht="30">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>14</v>
@@ -1278,26 +1272,6 @@
       </c>
       <c r="I14" s="3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="3">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3352,7 +3326,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>44</v>
@@ -3373,10 +3347,10 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="150">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
@@ -3394,10 +3368,10 @@
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="150">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -3415,10 +3389,10 @@
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="150">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
@@ -3436,10 +3410,10 @@
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="150">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -3457,10 +3431,10 @@
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="150">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
@@ -3478,10 +3452,10 @@
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="150">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
@@ -3499,10 +3473,10 @@
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="150">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
@@ -3520,7 +3494,7 @@
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>44</v>
@@ -3541,7 +3515,7 @@
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>71</v>
@@ -3562,7 +3536,7 @@
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>44</v>
@@ -3583,7 +3557,7 @@
     </row>
     <row r="12" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>71</v>
@@ -3604,10 +3578,10 @@
     </row>
     <row r="13" spans="1:7" s="3" customFormat="1" ht="165">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -3625,10 +3599,10 @@
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" ht="165">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
@@ -3646,7 +3620,7 @@
     </row>
     <row r="15" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>44</v>
@@ -3667,7 +3641,7 @@
     </row>
     <row r="16" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>71</v>
@@ -3688,10 +3662,10 @@
     </row>
     <row r="17" spans="1:7" s="3" customFormat="1" ht="165">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
@@ -3709,10 +3683,10 @@
     </row>
     <row r="18" spans="1:7" s="3" customFormat="1" ht="165">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>10</v>
@@ -3730,7 +3704,7 @@
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>44</v>
@@ -3751,7 +3725,7 @@
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>71</v>
@@ -3772,7 +3746,7 @@
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>44</v>
@@ -3793,7 +3767,7 @@
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>71</v>
@@ -3814,21 +3788,21 @@
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" ht="390">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>44</v>
@@ -3849,7 +3823,7 @@
     </row>
     <row r="25" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>71</v>
@@ -3870,21 +3844,21 @@
     </row>
     <row r="26" spans="1:7" s="3" customFormat="1" ht="375">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="3" customFormat="1" ht="135">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>44</v>
@@ -3920,7 +3894,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="240">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>19</v>
@@ -3941,10 +3915,10 @@
     </row>
     <row r="2" spans="1:7" ht="225">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
@@ -3962,10 +3936,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -3983,38 +3957,38 @@
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" ht="345">
       <c r="A11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="3" customFormat="1" ht="330">
       <c r="A12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="3" customFormat="1" ht="60">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -4032,30 +4006,30 @@
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" ht="270">
       <c r="A14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="3" customFormat="1" ht="270">
       <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>